<commit_message>
Individual Avg and PND times
</commit_message>
<xml_diff>
--- a/le15_p21_calls.xlsx
+++ b/le15_p21_calls.xlsx
@@ -5,25 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rat Pup call analysis\litter le15 fmr1\p21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rat Pup call analysis\Analysis pathway\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFE28A0-4C0F-4BE8-8992-781A7533C482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FDE5FE-E50E-422C-8B65-59B3F0D3DD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4410" yWindow="165" windowWidth="22185" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$168</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$168</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="80">
   <si>
     <t>File</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t>KO</t>
+  </si>
+  <si>
+    <t>Rat</t>
   </si>
 </sst>
 </file>
@@ -608,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S168"/>
+  <dimension ref="A1:T168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I139" workbookViewId="0">
-      <selection activeCell="U155" sqref="U155"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T136" sqref="T136:T168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -635,7 +638,7 @@
     <col min="18" max="18" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -693,8 +696,11 @@
       <c r="S1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="T1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -752,8 +758,11 @@
       <c r="S2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:19">
+      <c r="T2">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -811,8 +820,11 @@
       <c r="S3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="T3">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -870,8 +882,11 @@
       <c r="S4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="T4">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -929,8 +944,11 @@
       <c r="S5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="T5">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -988,8 +1006,11 @@
       <c r="S6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="T6">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1047,8 +1068,11 @@
       <c r="S7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="T7">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1106,8 +1130,11 @@
       <c r="S8" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="T8">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1165,8 +1192,11 @@
       <c r="S9" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="10" spans="1:19">
+      <c r="T9">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1224,8 +1254,11 @@
       <c r="S10" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="11" spans="1:19">
+      <c r="T10">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1283,8 +1316,11 @@
       <c r="S11" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="T11">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1342,8 +1378,11 @@
       <c r="S12" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="13" spans="1:19">
+      <c r="T12">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1401,8 +1440,11 @@
       <c r="S13" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="14" spans="1:19">
+      <c r="T13">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1460,8 +1502,11 @@
       <c r="S14" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="15" spans="1:19">
+      <c r="T14">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1519,8 +1564,11 @@
       <c r="S15" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="16" spans="1:19">
+      <c r="T15">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1578,8 +1626,11 @@
       <c r="S16" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="17" spans="1:19">
+      <c r="T16">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1637,8 +1688,11 @@
       <c r="S17" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:19">
+      <c r="T17">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1696,8 +1750,11 @@
       <c r="S18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:19">
+      <c r="T18">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1755,8 +1812,11 @@
       <c r="S19" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="20" spans="1:19">
+      <c r="T19">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1814,8 +1874,11 @@
       <c r="S20" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="21" spans="1:19">
+      <c r="T20">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1873,8 +1936,11 @@
       <c r="S21" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="22" spans="1:19">
+      <c r="T21">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1932,8 +1998,11 @@
       <c r="S22" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="23" spans="1:19">
+      <c r="T22">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1991,8 +2060,11 @@
       <c r="S23" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="24" spans="1:19">
+      <c r="T23">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2050,8 +2122,11 @@
       <c r="S24" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="25" spans="1:19">
+      <c r="T24">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -2109,8 +2184,11 @@
       <c r="S25" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="26" spans="1:19">
+      <c r="T25">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -2168,8 +2246,11 @@
       <c r="S26" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="27" spans="1:19">
+      <c r="T26">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -2227,8 +2308,11 @@
       <c r="S27" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="28" spans="1:19">
+      <c r="T27">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -2286,8 +2370,11 @@
       <c r="S28" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="29" spans="1:19">
+      <c r="T28">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -2345,8 +2432,11 @@
       <c r="S29" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="30" spans="1:19">
+      <c r="T29">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -2404,8 +2494,11 @@
       <c r="S30" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="31" spans="1:19">
+      <c r="T30">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -2463,8 +2556,11 @@
       <c r="S31" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="32" spans="1:19">
+      <c r="T31">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -2522,8 +2618,11 @@
       <c r="S32" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="33" spans="1:19">
+      <c r="T32">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -2581,8 +2680,11 @@
       <c r="S33" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="34" spans="1:19">
+      <c r="T33">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -2640,8 +2742,11 @@
       <c r="S34" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="35" spans="1:19">
+      <c r="T34">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -2699,8 +2804,11 @@
       <c r="S35" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="36" spans="1:19">
+      <c r="T35">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -2758,8 +2866,11 @@
       <c r="S36" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="37" spans="1:19">
+      <c r="T36">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -2817,8 +2928,11 @@
       <c r="S37" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="38" spans="1:19">
+      <c r="T37">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -2876,8 +2990,11 @@
       <c r="S38" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="39" spans="1:19">
+      <c r="T38">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -2935,8 +3052,11 @@
       <c r="S39" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="40" spans="1:19">
+      <c r="T39">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -2994,8 +3114,11 @@
       <c r="S40" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="41" spans="1:19">
+      <c r="T40">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -3053,8 +3176,11 @@
       <c r="S41" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="42" spans="1:19">
+      <c r="T41">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -3112,8 +3238,11 @@
       <c r="S42" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="43" spans="1:19">
+      <c r="T42">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -3171,8 +3300,11 @@
       <c r="S43" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="44" spans="1:19">
+      <c r="T43">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -3230,8 +3362,11 @@
       <c r="S44" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="45" spans="1:19">
+      <c r="T44">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -3289,8 +3424,11 @@
       <c r="S45" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="46" spans="1:19">
+      <c r="T45">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -3348,8 +3486,11 @@
       <c r="S46" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="47" spans="1:19">
+      <c r="T46">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -3407,8 +3548,11 @@
       <c r="S47" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="48" spans="1:19">
+      <c r="T47">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -3466,8 +3610,11 @@
       <c r="S48" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="49" spans="1:19">
+      <c r="T48">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -3525,8 +3672,11 @@
       <c r="S49" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="50" spans="1:19">
+      <c r="T49">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -3584,8 +3734,11 @@
       <c r="S50" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="51" spans="1:19">
+      <c r="T50">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -3643,8 +3796,11 @@
       <c r="S51" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="52" spans="1:19">
+      <c r="T51">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -3702,8 +3858,11 @@
       <c r="S52" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="53" spans="1:19">
+      <c r="T52">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -3761,8 +3920,11 @@
       <c r="S53" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="54" spans="1:19">
+      <c r="T53">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -3820,8 +3982,11 @@
       <c r="S54" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="55" spans="1:19">
+      <c r="T54">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -3879,8 +4044,11 @@
       <c r="S55" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="56" spans="1:19">
+      <c r="T55">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -3938,8 +4106,11 @@
       <c r="S56" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="57" spans="1:19">
+      <c r="T56">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -3997,8 +4168,11 @@
       <c r="S57" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="58" spans="1:19">
+      <c r="T57">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -4056,8 +4230,11 @@
       <c r="S58" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="59" spans="1:19">
+      <c r="T58">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -4115,8 +4292,11 @@
       <c r="S59" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="60" spans="1:19">
+      <c r="T59">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -4174,8 +4354,11 @@
       <c r="S60" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="61" spans="1:19">
+      <c r="T60">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -4233,8 +4416,11 @@
       <c r="S61" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="62" spans="1:19">
+      <c r="T61">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -4292,8 +4478,11 @@
       <c r="S62" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="63" spans="1:19">
+      <c r="T62">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -4351,8 +4540,11 @@
       <c r="S63" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="64" spans="1:19">
+      <c r="T63">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -4410,8 +4602,11 @@
       <c r="S64" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="65" spans="1:19">
+      <c r="T64">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -4469,8 +4664,11 @@
       <c r="S65" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="66" spans="1:19">
+      <c r="T65">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -4528,8 +4726,11 @@
       <c r="S66" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="67" spans="1:19">
+      <c r="T66">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -4587,8 +4788,11 @@
       <c r="S67" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="68" spans="1:19">
+      <c r="T67">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -4646,8 +4850,11 @@
       <c r="S68" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="69" spans="1:19">
+      <c r="T68">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20">
       <c r="A69" t="s">
         <v>5</v>
       </c>
@@ -4705,8 +4912,11 @@
       <c r="S69" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="70" spans="1:19">
+      <c r="T69">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -4764,8 +4974,11 @@
       <c r="S70" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="71" spans="1:19">
+      <c r="T70">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -4823,8 +5036,11 @@
       <c r="S71" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="72" spans="1:19">
+      <c r="T71">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -4882,8 +5098,11 @@
       <c r="S72" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="73" spans="1:19">
+      <c r="T72">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -4941,8 +5160,11 @@
       <c r="S73" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="74" spans="1:19">
+      <c r="T73">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -5000,8 +5222,11 @@
       <c r="S74" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="75" spans="1:19">
+      <c r="T74">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -5059,8 +5284,11 @@
       <c r="S75" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="76" spans="1:19">
+      <c r="T75">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -5118,8 +5346,11 @@
       <c r="S76" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="77" spans="1:19">
+      <c r="T76">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -5177,8 +5408,11 @@
       <c r="S77" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="78" spans="1:19">
+      <c r="T77">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -5236,8 +5470,11 @@
       <c r="S78" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="79" spans="1:19">
+      <c r="T78">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -5295,8 +5532,11 @@
       <c r="S79" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:19">
+      <c r="T79">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -5354,8 +5594,11 @@
       <c r="S80" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="1:19">
+      <c r="T80">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -5413,8 +5656,11 @@
       <c r="S81" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="82" spans="1:19">
+      <c r="T81">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -5472,8 +5718,11 @@
       <c r="S82" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="83" spans="1:19">
+      <c r="T82">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -5531,8 +5780,11 @@
       <c r="S83" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="84" spans="1:19">
+      <c r="T83">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -5590,8 +5842,11 @@
       <c r="S84" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="85" spans="1:19">
+      <c r="T84">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20">
       <c r="A85" t="s">
         <v>6</v>
       </c>
@@ -5649,8 +5904,11 @@
       <c r="S85" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="86" spans="1:19">
+      <c r="T85">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20">
       <c r="A86" t="s">
         <v>7</v>
       </c>
@@ -5708,8 +5966,11 @@
       <c r="S86" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="87" spans="1:19">
+      <c r="T86">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20">
       <c r="A87" t="s">
         <v>7</v>
       </c>
@@ -5767,8 +6028,11 @@
       <c r="S87" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="88" spans="1:19">
+      <c r="T87">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20">
       <c r="A88" t="s">
         <v>7</v>
       </c>
@@ -5826,8 +6090,11 @@
       <c r="S88" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="89" spans="1:19">
+      <c r="T88">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -5885,8 +6152,11 @@
       <c r="S89" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="90" spans="1:19">
+      <c r="T89">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20">
       <c r="A90" t="s">
         <v>7</v>
       </c>
@@ -5944,8 +6214,11 @@
       <c r="S90" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="91" spans="1:19">
+      <c r="T90">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20">
       <c r="A91" t="s">
         <v>7</v>
       </c>
@@ -6003,8 +6276,11 @@
       <c r="S91" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="92" spans="1:19">
+      <c r="T91">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20">
       <c r="A92" t="s">
         <v>7</v>
       </c>
@@ -6062,8 +6338,11 @@
       <c r="S92" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="93" spans="1:19">
+      <c r="T92">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20">
       <c r="A93" t="s">
         <v>7</v>
       </c>
@@ -6121,8 +6400,11 @@
       <c r="S93" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="94" spans="1:19">
+      <c r="T93">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20">
       <c r="A94" t="s">
         <v>7</v>
       </c>
@@ -6180,8 +6462,11 @@
       <c r="S94" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="95" spans="1:19">
+      <c r="T94">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20">
       <c r="A95" t="s">
         <v>7</v>
       </c>
@@ -6239,8 +6524,11 @@
       <c r="S95" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="96" spans="1:19">
+      <c r="T95">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -6298,8 +6586,11 @@
       <c r="S96" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="97" spans="1:19">
+      <c r="T96">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20">
       <c r="A97" t="s">
         <v>7</v>
       </c>
@@ -6357,8 +6648,11 @@
       <c r="S97" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="98" spans="1:19">
+      <c r="T97">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -6416,8 +6710,11 @@
       <c r="S98" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="99" spans="1:19">
+      <c r="T98">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -6475,8 +6772,11 @@
       <c r="S99" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="100" spans="1:19">
+      <c r="T99">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20">
       <c r="A100" t="s">
         <v>7</v>
       </c>
@@ -6534,8 +6834,11 @@
       <c r="S100" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="101" spans="1:19">
+      <c r="T100">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20">
       <c r="A101" t="s">
         <v>7</v>
       </c>
@@ -6593,8 +6896,11 @@
       <c r="S101" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="102" spans="1:19">
+      <c r="T101">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -6652,8 +6958,11 @@
       <c r="S102" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="103" spans="1:19">
+      <c r="T102">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20">
       <c r="A103" t="s">
         <v>7</v>
       </c>
@@ -6711,8 +7020,11 @@
       <c r="S103" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="104" spans="1:19">
+      <c r="T103">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20">
       <c r="A104" t="s">
         <v>7</v>
       </c>
@@ -6770,8 +7082,11 @@
       <c r="S104" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="105" spans="1:19">
+      <c r="T104">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20">
       <c r="A105" t="s">
         <v>7</v>
       </c>
@@ -6829,8 +7144,11 @@
       <c r="S105" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="106" spans="1:19">
+      <c r="T105">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20">
       <c r="A106" t="s">
         <v>7</v>
       </c>
@@ -6888,8 +7206,11 @@
       <c r="S106" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="107" spans="1:19">
+      <c r="T106">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20">
       <c r="A107" t="s">
         <v>7</v>
       </c>
@@ -6947,8 +7268,11 @@
       <c r="S107" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="108" spans="1:19">
+      <c r="T107">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20">
       <c r="A108" t="s">
         <v>7</v>
       </c>
@@ -7006,8 +7330,11 @@
       <c r="S108" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="109" spans="1:19">
+      <c r="T108">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20">
       <c r="A109" t="s">
         <v>7</v>
       </c>
@@ -7065,8 +7392,11 @@
       <c r="S109" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="110" spans="1:19">
+      <c r="T109">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20">
       <c r="A110" t="s">
         <v>7</v>
       </c>
@@ -7124,8 +7454,11 @@
       <c r="S110" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="111" spans="1:19">
+      <c r="T110">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20">
       <c r="A111" t="s">
         <v>7</v>
       </c>
@@ -7183,8 +7516,11 @@
       <c r="S111" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="112" spans="1:19">
+      <c r="T111">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20">
       <c r="A112" t="s">
         <v>7</v>
       </c>
@@ -7242,8 +7578,11 @@
       <c r="S112" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="113" spans="1:19">
+      <c r="T112">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20">
       <c r="A113" t="s">
         <v>7</v>
       </c>
@@ -7301,8 +7640,11 @@
       <c r="S113" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="114" spans="1:19">
+      <c r="T113">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20">
       <c r="A114" t="s">
         <v>8</v>
       </c>
@@ -7360,8 +7702,11 @@
       <c r="S114" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="115" spans="1:19">
+      <c r="T114">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20">
       <c r="A115" t="s">
         <v>8</v>
       </c>
@@ -7419,8 +7764,11 @@
       <c r="S115" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="116" spans="1:19">
+      <c r="T115">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20">
       <c r="A116" t="s">
         <v>8</v>
       </c>
@@ -7478,8 +7826,11 @@
       <c r="S116" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="117" spans="1:19">
+      <c r="T116">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20">
       <c r="A117" t="s">
         <v>8</v>
       </c>
@@ -7537,8 +7888,11 @@
       <c r="S117" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="118" spans="1:19">
+      <c r="T117">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20">
       <c r="A118" t="s">
         <v>8</v>
       </c>
@@ -7596,8 +7950,11 @@
       <c r="S118" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="119" spans="1:19">
+      <c r="T118">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20">
       <c r="A119" t="s">
         <v>8</v>
       </c>
@@ -7655,8 +8012,11 @@
       <c r="S119" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="120" spans="1:19">
+      <c r="T119">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20">
       <c r="A120" t="s">
         <v>8</v>
       </c>
@@ -7714,8 +8074,11 @@
       <c r="S120" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="121" spans="1:19">
+      <c r="T120">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20">
       <c r="A121" t="s">
         <v>8</v>
       </c>
@@ -7773,8 +8136,11 @@
       <c r="S121" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="122" spans="1:19">
+      <c r="T121">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20">
       <c r="A122" t="s">
         <v>8</v>
       </c>
@@ -7832,8 +8198,11 @@
       <c r="S122" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="123" spans="1:19">
+      <c r="T122">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20">
       <c r="A123" t="s">
         <v>8</v>
       </c>
@@ -7891,8 +8260,11 @@
       <c r="S123" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="124" spans="1:19">
+      <c r="T123">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20">
       <c r="A124" t="s">
         <v>8</v>
       </c>
@@ -7950,8 +8322,11 @@
       <c r="S124" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="125" spans="1:19">
+      <c r="T124">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20">
       <c r="A125" t="s">
         <v>8</v>
       </c>
@@ -8009,8 +8384,11 @@
       <c r="S125" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="126" spans="1:19">
+      <c r="T125">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20">
       <c r="A126" t="s">
         <v>8</v>
       </c>
@@ -8068,8 +8446,11 @@
       <c r="S126" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="127" spans="1:19">
+      <c r="T126">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20">
       <c r="A127" t="s">
         <v>8</v>
       </c>
@@ -8127,8 +8508,11 @@
       <c r="S127" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="128" spans="1:19">
+      <c r="T127">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20">
       <c r="A128" t="s">
         <v>8</v>
       </c>
@@ -8186,8 +8570,11 @@
       <c r="S128" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="129" spans="1:19">
+      <c r="T128">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20">
       <c r="A129" t="s">
         <v>8</v>
       </c>
@@ -8245,8 +8632,11 @@
       <c r="S129" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="130" spans="1:19">
+      <c r="T129">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20">
       <c r="A130" t="s">
         <v>8</v>
       </c>
@@ -8304,8 +8694,11 @@
       <c r="S130" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="131" spans="1:19">
+      <c r="T130">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20">
       <c r="A131" t="s">
         <v>8</v>
       </c>
@@ -8363,8 +8756,11 @@
       <c r="S131" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="132" spans="1:19">
+      <c r="T131">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20">
       <c r="A132" t="s">
         <v>8</v>
       </c>
@@ -8422,8 +8818,11 @@
       <c r="S132" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="133" spans="1:19">
+      <c r="T132">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20">
       <c r="A133" t="s">
         <v>8</v>
       </c>
@@ -8481,8 +8880,11 @@
       <c r="S133" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="134" spans="1:19">
+      <c r="T133">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20">
       <c r="A134" t="s">
         <v>8</v>
       </c>
@@ -8540,8 +8942,11 @@
       <c r="S134" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="135" spans="1:19">
+      <c r="T134">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20">
       <c r="A135" t="s">
         <v>9</v>
       </c>
@@ -8599,8 +9004,11 @@
       <c r="S135" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="136" spans="1:19">
+      <c r="T135">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20">
       <c r="A136" t="s">
         <v>9</v>
       </c>
@@ -8658,8 +9066,11 @@
       <c r="S136" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="137" spans="1:19">
+      <c r="T136">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20">
       <c r="A137" t="s">
         <v>9</v>
       </c>
@@ -8717,8 +9128,11 @@
       <c r="S137" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="138" spans="1:19">
+      <c r="T137">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20">
       <c r="A138" t="s">
         <v>9</v>
       </c>
@@ -8776,8 +9190,11 @@
       <c r="S138" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="139" spans="1:19">
+      <c r="T138">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20">
       <c r="A139" t="s">
         <v>9</v>
       </c>
@@ -8835,8 +9252,11 @@
       <c r="S139" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="140" spans="1:19">
+      <c r="T139">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20">
       <c r="A140" t="s">
         <v>9</v>
       </c>
@@ -8894,8 +9314,11 @@
       <c r="S140" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="141" spans="1:19">
+      <c r="T140">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20">
       <c r="A141" t="s">
         <v>9</v>
       </c>
@@ -8953,8 +9376,11 @@
       <c r="S141" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="142" spans="1:19">
+      <c r="T141">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20">
       <c r="A142" t="s">
         <v>9</v>
       </c>
@@ -9012,8 +9438,11 @@
       <c r="S142" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="143" spans="1:19">
+      <c r="T142">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20">
       <c r="A143" t="s">
         <v>9</v>
       </c>
@@ -9071,8 +9500,11 @@
       <c r="S143" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="144" spans="1:19">
+      <c r="T143">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20">
       <c r="A144" t="s">
         <v>9</v>
       </c>
@@ -9130,8 +9562,11 @@
       <c r="S144" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="145" spans="1:19">
+      <c r="T144">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20">
       <c r="A145" t="s">
         <v>9</v>
       </c>
@@ -9189,8 +9624,11 @@
       <c r="S145" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="146" spans="1:19">
+      <c r="T145">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20">
       <c r="A146" t="s">
         <v>9</v>
       </c>
@@ -9248,8 +9686,11 @@
       <c r="S146" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="147" spans="1:19">
+      <c r="T146">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="147" spans="1:20">
       <c r="A147" t="s">
         <v>9</v>
       </c>
@@ -9307,8 +9748,11 @@
       <c r="S147" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="148" spans="1:19">
+      <c r="T147">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="148" spans="1:20">
       <c r="A148" t="s">
         <v>9</v>
       </c>
@@ -9366,8 +9810,11 @@
       <c r="S148" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="149" spans="1:19">
+      <c r="T148">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="149" spans="1:20">
       <c r="A149" t="s">
         <v>9</v>
       </c>
@@ -9425,8 +9872,11 @@
       <c r="S149" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="150" spans="1:19">
+      <c r="T149">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="150" spans="1:20">
       <c r="A150" t="s">
         <v>9</v>
       </c>
@@ -9484,8 +9934,11 @@
       <c r="S150" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="151" spans="1:19">
+      <c r="T150">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="151" spans="1:20">
       <c r="A151" t="s">
         <v>9</v>
       </c>
@@ -9543,8 +9996,11 @@
       <c r="S151" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="152" spans="1:19">
+      <c r="T151">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="152" spans="1:20">
       <c r="A152" t="s">
         <v>9</v>
       </c>
@@ -9602,8 +10058,11 @@
       <c r="S152" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="153" spans="1:19">
+      <c r="T152">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="153" spans="1:20">
       <c r="A153" t="s">
         <v>9</v>
       </c>
@@ -9661,8 +10120,11 @@
       <c r="S153" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="154" spans="1:19">
+      <c r="T153">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="154" spans="1:20">
       <c r="A154" t="s">
         <v>9</v>
       </c>
@@ -9720,8 +10182,11 @@
       <c r="S154" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="155" spans="1:19">
+      <c r="T154">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="155" spans="1:20">
       <c r="A155" t="s">
         <v>9</v>
       </c>
@@ -9779,8 +10244,11 @@
       <c r="S155" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="156" spans="1:19">
+      <c r="T155">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="156" spans="1:20">
       <c r="A156" t="s">
         <v>9</v>
       </c>
@@ -9838,8 +10306,11 @@
       <c r="S156" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="157" spans="1:19">
+      <c r="T156">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="157" spans="1:20">
       <c r="A157" t="s">
         <v>9</v>
       </c>
@@ -9897,8 +10368,11 @@
       <c r="S157" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="158" spans="1:19">
+      <c r="T157">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="158" spans="1:20">
       <c r="A158" t="s">
         <v>10</v>
       </c>
@@ -9956,8 +10430,11 @@
       <c r="S158" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="159" spans="1:19">
+      <c r="T158">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="159" spans="1:20">
       <c r="A159" t="s">
         <v>10</v>
       </c>
@@ -10015,8 +10492,11 @@
       <c r="S159" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="160" spans="1:19">
+      <c r="T159">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="160" spans="1:20">
       <c r="A160" t="s">
         <v>10</v>
       </c>
@@ -10074,8 +10554,11 @@
       <c r="S160" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="161" spans="1:19">
+      <c r="T160">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="161" spans="1:20">
       <c r="A161" t="s">
         <v>10</v>
       </c>
@@ -10133,8 +10616,11 @@
       <c r="S161" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="162" spans="1:19">
+      <c r="T161">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="162" spans="1:20">
       <c r="A162" t="s">
         <v>10</v>
       </c>
@@ -10192,8 +10678,11 @@
       <c r="S162" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="163" spans="1:19">
+      <c r="T162">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="163" spans="1:20">
       <c r="A163" t="s">
         <v>10</v>
       </c>
@@ -10251,8 +10740,11 @@
       <c r="S163" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="164" spans="1:19">
+      <c r="T163">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="164" spans="1:20">
       <c r="A164" t="s">
         <v>10</v>
       </c>
@@ -10310,8 +10802,11 @@
       <c r="S164" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="165" spans="1:19">
+      <c r="T164">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="165" spans="1:20">
       <c r="A165" t="s">
         <v>10</v>
       </c>
@@ -10369,8 +10864,11 @@
       <c r="S165" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="166" spans="1:19">
+      <c r="T165">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="166" spans="1:20">
       <c r="A166" t="s">
         <v>10</v>
       </c>
@@ -10428,8 +10926,11 @@
       <c r="S166" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="167" spans="1:19">
+      <c r="T166">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="167" spans="1:20">
       <c r="A167" t="s">
         <v>10</v>
       </c>
@@ -10487,8 +10988,11 @@
       <c r="S167" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="168" spans="1:19">
+      <c r="T167">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="168" spans="1:20">
       <c r="A168" t="s">
         <v>10</v>
       </c>
@@ -10546,8 +11050,12 @@
       <c r="S168" t="s">
         <v>78</v>
       </c>
+      <c r="T168">
+        <v>568</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:T168" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>